<commit_message>
FOLDER STRUCTURE AND FILE MAPPINGS UPDATED
</commit_message>
<xml_diff>
--- a/DOCUMENTS/A_DATA_MAPPING/_01_Scoping.xlsx
+++ b/DOCUMENTS/A_DATA_MAPPING/_01_Scoping.xlsx
@@ -7,17 +7,18 @@
     <workbookView xWindow="720" yWindow="330" windowWidth="22755" windowHeight="9750"/>
   </bookViews>
   <sheets>
-    <sheet name="Employee_Master" sheetId="1" r:id="rId1"/>
-    <sheet name="Acerno_Cache_XXXXX" sheetId="4" state="veryHidden" r:id="rId2"/>
-    <sheet name="Payroll" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="General" sheetId="3" r:id="rId1"/>
+    <sheet name="Employee_Master" sheetId="1" r:id="rId2"/>
+    <sheet name="Acerno_Cache_XXXXX" sheetId="4" state="veryHidden" r:id="rId3"/>
+    <sheet name="Payroll" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="91">
   <si>
     <t>EM001</t>
   </si>
@@ -656,6 +657,60 @@
   </si>
   <si>
     <t>Employees with Blank TFN and or 11111111 and tax is not the highest marginal rate (over 28 days for AUS)</t>
+  </si>
+  <si>
+    <t>What is your source system for Employee Master Data?</t>
+  </si>
+  <si>
+    <t>What is your source system for Payroll Data?</t>
+  </si>
+  <si>
+    <t>How do you proposed we access this data?</t>
+  </si>
+  <si>
+    <t>Employee Master Data:</t>
+  </si>
+  <si>
+    <t>Payroll Data:</t>
+  </si>
+  <si>
+    <t>Question:</t>
+  </si>
+  <si>
+    <t>SAP / Chris21</t>
+  </si>
+  <si>
+    <t>Guidance / Examples:</t>
+  </si>
+  <si>
+    <t>Direct Link / ODBC</t>
+  </si>
+  <si>
+    <t>ODBC, Flat Files, PDF Reports, etc</t>
+  </si>
+  <si>
+    <t>Chris21</t>
+  </si>
+  <si>
+    <t>Information is related to the following EVA Areas:</t>
+  </si>
+  <si>
+    <t>Data Downloads and Data Preparation</t>
+  </si>
+  <si>
+    <t>Reponses:</t>
+  </si>
+  <si>
+    <t>How would we identify inactive / terminated employees</t>
+  </si>
+  <si>
+    <t>How would we identify temp / casual employees</t>
+  </si>
+  <si>
+    <t>How woud we identify permanent staff</t>
+  </si>
+  <si>
+    <t>Does the payroll run fortnightly and monthly?</t>
   </si>
 </sst>
 </file>
@@ -891,27 +946,51 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -923,30 +1002,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1249,10 +1304,119 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:E19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="50.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" customWidth="1"/>
+    <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" t="s">
+        <v>82</v>
+      </c>
+      <c r="E18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1303,58 +1467,58 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8" t="s">
+      <c r="A8" s="18"/>
+      <c r="B8" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8" t="s">
+      <c r="A9" s="18"/>
+      <c r="B9" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8" t="s">
+      <c r="A10" s="18"/>
+      <c r="B10" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8" t="s">
+      <c r="A11" s="18"/>
+      <c r="B11" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8" t="s">
+      <c r="A12" s="18"/>
+      <c r="B12" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8" t="s">
+      <c r="A13" s="18"/>
+      <c r="B13" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8" t="s">
+      <c r="A14" s="18"/>
+      <c r="B14" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="9"/>
-      <c r="B15" s="10" t="s">
+      <c r="A15" s="19"/>
+      <c r="B15" s="7" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1367,16 +1531,16 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="6" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1389,7 +1553,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="17" t="s">
         <v>27</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -1397,39 +1561,39 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="8" t="s">
+      <c r="A21" s="18"/>
+      <c r="B21" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="9"/>
-      <c r="B22" s="8" t="s">
+      <c r="A22" s="19"/>
+      <c r="B22" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="8" t="s">
+      <c r="A24" s="18"/>
+      <c r="B24" s="6" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="9"/>
-      <c r="B25" s="10" t="s">
+      <c r="A25" s="19"/>
+      <c r="B25" s="7" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="17" t="s">
         <v>35</v>
       </c>
       <c r="B26" s="4" t="s">
@@ -1437,46 +1601,46 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="8" t="s">
+      <c r="A27" s="18"/>
+      <c r="B27" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" s="8" t="s">
+      <c r="A28" s="18"/>
+      <c r="B28" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="9"/>
-      <c r="B29" s="8" t="s">
+      <c r="A29" s="19"/>
+      <c r="B29" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="8" t="s">
+      <c r="A31" s="18"/>
+      <c r="B31" s="6" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="B32" s="8" t="s">
+      <c r="A32" s="18"/>
+      <c r="B32" s="6" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="9"/>
-      <c r="B33" s="10" t="s">
+      <c r="A33" s="19"/>
+      <c r="B33" s="7" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1489,33 +1653,33 @@
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="5" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="9"/>
-      <c r="B36" s="10" t="s">
+      <c r="A36" s="19"/>
+      <c r="B36" s="7" t="s">
         <v>49</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A35:A36"/>
     <mergeCell ref="A7:A15"/>
     <mergeCell ref="A20:A22"/>
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="A26:A29"/>
     <mergeCell ref="A30:A33"/>
-    <mergeCell ref="A35:A36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1523,14 +1687,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="23"/>
+    <col min="1" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
@@ -1545,100 +1709,100 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="21"/>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="15"/>
+      <c r="B2" s="23"/>
     </row>
     <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="10" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="12" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="10" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="12" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
-      <c r="B7" s="20" t="s">
+      <c r="A7" s="19"/>
+      <c r="B7" s="13" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="10" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="12" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="10" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="12" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="10" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="15" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1652,11 +1816,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>